<commit_message>
fix some case data issue
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/ddl/sql_ddl_cases_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/ddl/sql_ddl_cases_btree.xlsx
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
change dingo connection by Druid connection pool
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/ddl/sql_ddl_cases_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/ddl/sql_ddl_cases_btree.xlsx
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>